<commit_message>
Minor updates to documents
Just so that I can sync
</commit_message>
<xml_diff>
--- a/Meeting Details/Burn Down Chart.xlsx
+++ b/Meeting Details/Burn Down Chart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Timeline (day no.)</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Actual tasks rem.</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -68,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -182,7 +186,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1'!$B$1</c:f>
+              <c:f>'Sprint 1'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -217,7 +221,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$B$2:$B$21</c:f>
+              <c:f>'Sprint 1'!$C$2:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -296,7 +300,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 1'!$C$1</c:f>
+              <c:f>'Sprint 1'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -331,7 +335,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$C$2:$C$21</c:f>
+              <c:f>'Sprint 1'!$D$2:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1232,13 +1236,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -1566,212 +1570,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>42982</v>
+      </c>
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>34</v>
       </c>
       <c r="C2">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="D2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42983</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <f>ROUND($B$2 - ($B$2/20*A2) - 2, 0)</f>
+      <c r="C3">
+        <f>ROUND($C$2 - ($C$2/20*B2) - 2, 0)</f>
         <v>30</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42984</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <f t="shared" ref="B4:B21" si="0">ROUND($B$2 - ($B$2/20*A3) - 2, 0)</f>
+      <c r="C4">
+        <f t="shared" ref="C4:C21" si="0">ROUND($C$2 - ($C$2/20*B3) - 2, 0)</f>
         <v>29</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42985</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42986</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42989</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42990</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42991</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42992</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42993</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>42996</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>42997</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>42998</v>
+      </c>
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>42999</v>
+      </c>
+      <c r="B15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43000</v>
+      </c>
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43003</v>
+      </c>
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43004</v>
+      </c>
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43005</v>
+      </c>
+      <c r="B19">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43006</v>
+      </c>
+      <c r="B20">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43007</v>
+      </c>
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Text if no reviews written + burndown chart update
</commit_message>
<xml_diff>
--- a/Meeting Details/Burn Down Chart.xlsx
+++ b/Meeting Details/Burn Down Chart.xlsx
@@ -1016,6 +1016,36 @@
                 <c:pt idx="7">
                   <c:v>23</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3313,6 +3343,9 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -3325,6 +3358,9 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -3337,6 +3373,9 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
+      <c r="D12">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -3349,6 +3388,9 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
+      <c r="D13">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -3361,6 +3403,9 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -3373,6 +3418,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -3385,8 +3433,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43038</v>
       </c>
@@ -3397,8 +3448,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43039</v>
       </c>
@@ -3409,8 +3463,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43040</v>
       </c>
@@ -3421,8 +3478,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43041</v>
       </c>
@@ -3434,7 +3494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43042</v>
       </c>

</xml_diff>

<commit_message>
Burn down chart finished
</commit_message>
<xml_diff>
--- a/Meeting Details/Burn Down Chart.xlsx
+++ b/Meeting Details/Burn Down Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougm\OneDrive\BIT - Semester 4\IFB299 App Design and Development\Project\ifb299\Meeting Details\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/94f4f8f9765bfce3/BIT - Semester 4/IFB299 App Design and Development/Project/ifb299/Meeting Details/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -921,21 +921,15 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1041,10 +1035,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3430,8 +3424,7 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -3445,8 +3438,7 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <v>7</v>
@@ -3460,11 +3452,10 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D18">
         <v>4</v>
-      </c>
-      <c r="D18">
-        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3475,36 +3466,17 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>43041</v>
-      </c>
-      <c r="B20">
-        <v>19</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="A20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>43042</v>
-      </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>